<commit_message>
bot to telegram plus word docs
</commit_message>
<xml_diff>
--- a/wordDocs/Gantt chart.xlsx
+++ b/wordDocs/Gantt chart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="880" windowWidth="24960" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="-24000" yWindow="-18300" windowWidth="24960" windowHeight="14740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,10 +74,10 @@
     <t>Optimizing models</t>
   </si>
   <si>
-    <t>Gathering training data for machine learning</t>
-  </si>
-  <si>
     <t xml:space="preserve">Train models on new functionality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gathering training data </t>
   </si>
 </sst>
 </file>
@@ -487,32 +487,33 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.5" customWidth="1"/>
-    <col min="2" max="2" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3" customWidth="1"/>
     <col min="3" max="3" width="2.83203125" customWidth="1"/>
-    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="7" width="4" customWidth="1"/>
-    <col min="8" max="9" width="3.83203125" customWidth="1"/>
-    <col min="10" max="10" width="3.6640625" customWidth="1"/>
-    <col min="11" max="11" width="3.5" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" customWidth="1"/>
-    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="10" width="2.83203125" customWidth="1"/>
+    <col min="11" max="12" width="3.1640625" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" customWidth="1"/>
     <col min="14" max="14" width="3.33203125" customWidth="1"/>
-    <col min="15" max="15" width="6.5" customWidth="1"/>
-    <col min="16" max="16" width="4.5" customWidth="1"/>
-    <col min="17" max="17" width="4.33203125" customWidth="1"/>
-    <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="19" max="20" width="3.5" customWidth="1"/>
-    <col min="21" max="21" width="4" customWidth="1"/>
-    <col min="22" max="22" width="3.5" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" customWidth="1"/>
+    <col min="16" max="16" width="3" customWidth="1"/>
+    <col min="17" max="17" width="3.1640625" customWidth="1"/>
+    <col min="18" max="18" width="3" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" customWidth="1"/>
+    <col min="20" max="20" width="3.5" customWidth="1"/>
+    <col min="21" max="21" width="2.83203125" customWidth="1"/>
+    <col min="22" max="22" width="2.33203125" customWidth="1"/>
     <col min="23" max="23" width="5.33203125" customWidth="1"/>
-    <col min="24" max="24" width="4" customWidth="1"/>
+    <col min="24" max="24" width="3.33203125" customWidth="1"/>
     <col min="25" max="25" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -684,7 +685,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -887,7 +888,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>

</xml_diff>